<commit_message>
final touches before spring sem
</commit_message>
<xml_diff>
--- a/msda_saves.xlsx
+++ b/msda_saves.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yash Lal\Desktop\Microbial Vector Field Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2858F4E4-6A11-4AEA-A711-3AC37F07EC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF88004-70C1-41CB-A2D4-7578CA8DB0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>[0.11775572597980499, 0.0343063585460186, 0.10792648792266846, 0.020337529480457306, 0.03209932893514633, 0.02721654810011387, 0.1804841011762619, 0.26857760548591614, 0.2646385431289673, 0.13413883745670319, 0.1187481066212058]</t>
   </si>
@@ -52,6 +52,36 @@
   </si>
   <si>
     <t>[0.11710374802350998, 0.034129686653614044, 0.10848668962717056, 0.03047170676290989, 0.031868498772382736, 0.026713870465755463, 0.19840358197689056, 0.271660178899765, 0.2961809039115906, 0.13251961767673492, 0.12475384827703237]</t>
+  </si>
+  <si>
+    <t>NM(64)</t>
+  </si>
+  <si>
+    <t>[0.12058988213539124, 0.03436800464987755, 0.10352993756532669, 0.02030286379158497, 0.03217571601271629, 0.02710207737982273, 0.18644094467163086, 0.3134118318557739, 0.25580230355262756, 0.13114772737026215, 0.1224871288985014]</t>
+  </si>
+  <si>
+    <t>NM+4CM(rect)(64)</t>
+  </si>
+  <si>
+    <t>[0.11653576046228409, 0.03403253108263016, 0.10798562318086624, 0.021862655878067017, 0.03326644003391266, 0.027488116174936295, 0.20256248116493225, 0.238773375749588, 0.23526504635810852, 0.1368890106678009, 0.11546610407531262]</t>
+  </si>
+  <si>
+    <t>NM+4CM(custom)(64)</t>
+  </si>
+  <si>
+    <t>[0.11634423583745956, 0.03415555879473686, 0.10137994587421417, 0.0216276366263628, 0.032765522599220276, 0.027110232040286064, 0.18748654425144196, 0.23630554974079132, 0.24979417026042938, 0.13126122951507568, 0.1138230625540018]</t>
+  </si>
+  <si>
+    <t>NM+4MixUp(64)</t>
+  </si>
+  <si>
+    <t>[0.11625339835882187, 0.033972881734371185, 0.10771539062261581, 0.024174481630325317, 0.03213963657617569, 0.027086645364761353, 0.17631056904792786, 0.3103159964084625, 0.2537173330783844, 0.12410194426774979, 0.12057882770895959]</t>
+  </si>
+  <si>
+    <t>[0.11612879484891891, 0.03450104221701622, 0.1083734780550003, 0.027244193479418755, 0.032124631106853485, 0.026846332475543022, 0.19984659552574158, 0.25128018856048584, 0.22460828721523285, 0.13065199553966522, 0.11516055390238762]</t>
+  </si>
+  <si>
+    <t>NM+9CM(custom)(64)</t>
   </si>
 </sst>
 </file>
@@ -369,15 +399,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -413,6 +443,46 @@
         <v>0.124753848277032</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.122487128898501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>0.11546610407531201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0.113823062554001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>0.120578827708959</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>0.115160553902387</v>
+      </c>
+    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
         <v>7</v>
@@ -436,6 +506,31 @@
     <row r="20" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>